<commit_message>
added files to git ignore and converted temp resistance to voltage
</commit_message>
<xml_diff>
--- a/Temp Equations.xlsx
+++ b/Temp Equations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Helen\Documents\GitHub\Embedded Labs\introtoembedded-f18-milestone2-nano-tech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{761B2372-3A0E-4AC7-AA97-C36274A8D669}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{72871C77-90B0-4F3D-9636-72AB5933BD8B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="12160" xr2:uid="{3E3DEB7C-21E9-4463-883A-51990C89E091}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="179017"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Temperture</t>
   </si>
@@ -92,6 +91,9 @@
   </si>
   <si>
     <t>y=-0.0008x+25.311</t>
+  </si>
+  <si>
+    <t>Voltage Equavient</t>
   </si>
 </sst>
 </file>
@@ -169,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -178,6 +180,7 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -756,7 +759,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$N$2:$N$33</c:f>
+              <c:f>Sheet1!$P$2:$P$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -858,7 +861,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$O$2:$O$33</c:f>
+              <c:f>Sheet1!$Q$2:$Q$33</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
@@ -2305,15 +2308,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>434975</xdr:colOff>
+      <xdr:colOff>111125</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>98425</xdr:rowOff>
+      <xdr:rowOff>34925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>130175</xdr:colOff>
+      <xdr:colOff>415925</xdr:colOff>
       <xdr:row>32</xdr:row>
-      <xdr:rowOff>79375</xdr:rowOff>
+      <xdr:rowOff>15875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2638,41 +2641,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{727EDA6D-1792-45E4-9ABC-7EE04BE1361E}">
-  <dimension ref="A1:W32"/>
+  <dimension ref="A1:Y32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+      <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12.81640625" customWidth="1"/>
     <col min="4" max="4" width="17.7265625" customWidth="1"/>
-    <col min="14" max="14" width="10.453125" customWidth="1"/>
-    <col min="16" max="16" width="2" customWidth="1"/>
-    <col min="17" max="17" width="2.26953125" customWidth="1"/>
+    <col min="15" max="15" width="16.1796875" customWidth="1"/>
+    <col min="16" max="16" width="10.453125" customWidth="1"/>
     <col min="18" max="18" width="2" customWidth="1"/>
-    <col min="19" max="19" width="1.81640625" customWidth="1"/>
-    <col min="20" max="20" width="2.08984375" customWidth="1"/>
+    <col min="19" max="19" width="2.26953125" customWidth="1"/>
+    <col min="20" max="20" width="2" customWidth="1"/>
     <col min="21" max="21" width="1.81640625" customWidth="1"/>
-    <col min="22" max="22" width="1.453125" customWidth="1"/>
+    <col min="22" max="22" width="2.08984375" customWidth="1"/>
+    <col min="23" max="23" width="1.81640625" customWidth="1"/>
+    <col min="24" max="24" width="1.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -2682,15 +2689,19 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
-      <c r="N2">
+      <c r="O2" s="8">
+        <f>(3.3*P2)/(10000+P2)</f>
+        <v>2.5245147342200496</v>
+      </c>
+      <c r="P2">
         <v>32554</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>0</v>
       </c>
-      <c r="V2" s="7"/>
+      <c r="X2" s="7"/>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>5</v>
       </c>
@@ -2700,18 +2711,22 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="N3">
+      <c r="O3" s="8">
+        <f t="shared" ref="O3:O32" si="0">(3.3*P3)/(10000+P3)</f>
+        <v>2.3661874982314157</v>
+      </c>
+      <c r="P3">
         <v>25339</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>5</v>
       </c>
-      <c r="V3" s="7"/>
-      <c r="W3" t="s">
+      <c r="X3" s="7"/>
+      <c r="Y3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>10</v>
       </c>
@@ -2721,16 +2736,20 @@
       <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="N4">
+      <c r="O4" s="8">
+        <f t="shared" si="0"/>
+        <v>2.1952865559721477</v>
+      </c>
+      <c r="P4">
         <v>19872</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>10</v>
       </c>
-      <c r="U4" s="6"/>
-      <c r="V4" s="7"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="7"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>15</v>
       </c>
@@ -2740,33 +2759,41 @@
       <c r="D5" t="s">
         <v>11</v>
       </c>
-      <c r="N5">
+      <c r="O5" s="8">
+        <f t="shared" si="0"/>
+        <v>2.0158533738034086</v>
+      </c>
+      <c r="P5">
         <v>15698</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>15</v>
       </c>
-      <c r="U5" s="6"/>
+      <c r="W5" s="6"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>20</v>
       </c>
       <c r="B6">
         <v>12488</v>
       </c>
-      <c r="N6">
+      <c r="O6" s="8">
+        <f t="shared" si="0"/>
+        <v>1.8325506937033083</v>
+      </c>
+      <c r="P6">
         <v>12488</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>20</v>
       </c>
-      <c r="U6" s="6"/>
-      <c r="V6" t="s">
+      <c r="W6" s="6"/>
+      <c r="X6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>25</v>
       </c>
@@ -2776,16 +2803,20 @@
       <c r="D7" t="s">
         <v>8</v>
       </c>
-      <c r="N7">
+      <c r="O7" s="8">
+        <f t="shared" si="0"/>
+        <v>1.65</v>
+      </c>
+      <c r="P7">
         <v>10000</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>25</v>
       </c>
-      <c r="T7" s="5"/>
-      <c r="U7" s="6"/>
+      <c r="V7" s="5"/>
+      <c r="W7" s="6"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>30</v>
       </c>
@@ -2795,33 +2826,41 @@
       <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="N8">
+      <c r="O8" s="8">
+        <f t="shared" si="0"/>
+        <v>1.4726562932609777</v>
+      </c>
+      <c r="P8">
         <v>8059</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>30</v>
       </c>
-      <c r="T8" s="5"/>
+      <c r="V8" s="5"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>35</v>
       </c>
       <c r="B9">
         <v>6535</v>
       </c>
-      <c r="N9">
+      <c r="O9" s="8">
+        <f t="shared" si="0"/>
+        <v>1.3042334442092531</v>
+      </c>
+      <c r="P9">
         <v>6535</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>35</v>
       </c>
-      <c r="T9" s="5"/>
-      <c r="U9" t="s">
+      <c r="V9" s="5"/>
+      <c r="W9" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>40</v>
       </c>
@@ -2831,15 +2870,19 @@
       <c r="D10" t="s">
         <v>6</v>
       </c>
-      <c r="N10">
+      <c r="O10" s="8">
+        <f t="shared" si="0"/>
+        <v>1.147358121330724</v>
+      </c>
+      <c r="P10">
         <v>5330</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>40</v>
       </c>
-      <c r="T10" s="5"/>
+      <c r="V10" s="5"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>45</v>
       </c>
@@ -2849,64 +2892,80 @@
       <c r="D11" t="s">
         <v>7</v>
       </c>
-      <c r="N11">
+      <c r="O11" s="8">
+        <f t="shared" si="0"/>
+        <v>1.0038686334539382</v>
+      </c>
+      <c r="P11">
         <v>4372</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>45</v>
       </c>
-      <c r="S11" s="1"/>
-      <c r="T11" s="5"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="5"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>50</v>
       </c>
       <c r="B12">
         <v>3605</v>
       </c>
-      <c r="N12">
+      <c r="O12" s="8">
+        <f t="shared" si="0"/>
+        <v>0.87442116868798236</v>
+      </c>
+      <c r="P12">
         <v>3605</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>50</v>
       </c>
-      <c r="S12" s="1"/>
+      <c r="U12" s="1"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>55</v>
       </c>
       <c r="B13">
         <v>2989</v>
       </c>
-      <c r="N13">
+      <c r="O13" s="8">
+        <f t="shared" si="0"/>
+        <v>0.75938871352683035</v>
+      </c>
+      <c r="P13">
         <v>2989</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>55</v>
       </c>
-      <c r="S13" s="1"/>
-      <c r="T13" t="s">
+      <c r="U13" s="1"/>
+      <c r="V13" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>60</v>
       </c>
       <c r="B14">
         <v>2490</v>
       </c>
-      <c r="N14">
+      <c r="O14" s="8">
+        <f t="shared" si="0"/>
+        <v>0.65788630904723777</v>
+      </c>
+      <c r="P14">
         <v>2490</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>60</v>
       </c>
-      <c r="S14" s="1"/>
+      <c r="U14" s="1"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>65</v>
       </c>
@@ -2916,15 +2975,19 @@
       <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="N15">
+      <c r="O15" s="8">
+        <f t="shared" si="0"/>
+        <v>0.5691161866931479</v>
+      </c>
+      <c r="P15">
         <v>2084</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>65</v>
       </c>
-      <c r="S15" s="1"/>
+      <c r="U15" s="1"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>70</v>
       </c>
@@ -2934,95 +2997,119 @@
       <c r="D16" t="s">
         <v>5</v>
       </c>
-      <c r="N16">
+      <c r="O16" s="8">
+        <f t="shared" si="0"/>
+        <v>0.49220624521398787</v>
+      </c>
+      <c r="P16">
         <v>1753</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>70</v>
       </c>
-      <c r="R16" s="4"/>
-      <c r="S16" s="1"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="1"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>75</v>
       </c>
       <c r="B17">
         <v>1481</v>
       </c>
-      <c r="N17">
+      <c r="O17" s="8">
+        <f t="shared" si="0"/>
+        <v>0.42568591586098775</v>
+      </c>
+      <c r="P17">
         <v>1481</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>75</v>
       </c>
-      <c r="R17" s="4"/>
+      <c r="T17" s="4"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>80</v>
       </c>
       <c r="B18">
         <v>1256</v>
       </c>
-      <c r="N18">
+      <c r="O18" s="8">
+        <f t="shared" si="0"/>
+        <v>0.36823027718550111</v>
+      </c>
+      <c r="P18">
         <v>1256</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>80</v>
       </c>
-      <c r="R18" s="4"/>
-      <c r="S18" t="s">
+      <c r="T18" s="4"/>
+      <c r="U18" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>85</v>
       </c>
       <c r="B19">
         <v>1070</v>
       </c>
-      <c r="N19">
+      <c r="O19" s="8">
+        <f t="shared" si="0"/>
+        <v>0.318970189701897</v>
+      </c>
+      <c r="P19">
         <v>1070</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>85</v>
       </c>
-      <c r="R19" s="4"/>
+      <c r="T19" s="4"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>90</v>
       </c>
       <c r="B20">
         <v>915.4</v>
       </c>
-      <c r="N20">
+      <c r="O20" s="8">
+        <f t="shared" si="0"/>
+        <v>0.27674844714806601</v>
+      </c>
+      <c r="P20">
         <v>915.4</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>90</v>
       </c>
-      <c r="R20" s="4"/>
+      <c r="T20" s="4"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>95</v>
       </c>
       <c r="B21">
         <v>786</v>
       </c>
-      <c r="N21">
+      <c r="O21" s="8">
+        <f t="shared" si="0"/>
+        <v>0.24047839792323381</v>
+      </c>
+      <c r="P21">
         <v>786</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>95</v>
       </c>
-      <c r="Q21" s="3"/>
-      <c r="R21" s="4"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="4"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>100</v>
       </c>
@@ -3032,15 +3119,19 @@
       <c r="D22" t="s">
         <v>2</v>
       </c>
-      <c r="N22">
+      <c r="O22" s="8">
+        <f t="shared" si="0"/>
+        <v>0.2093310106487595</v>
+      </c>
+      <c r="P22">
         <v>677.3</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>100</v>
       </c>
-      <c r="Q22" s="3"/>
+      <c r="S22" s="3"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>105</v>
       </c>
@@ -3050,155 +3141,195 @@
       <c r="D23" t="s">
         <v>3</v>
       </c>
-      <c r="N23">
+      <c r="O23" s="8">
+        <f t="shared" si="0"/>
+        <v>0.18258688608216744</v>
+      </c>
+      <c r="P23">
         <v>585.70000000000005</v>
       </c>
-      <c r="O23">
+      <c r="Q23">
         <v>105</v>
       </c>
-      <c r="Q23" s="3"/>
-      <c r="R23" t="s">
+      <c r="S23" s="3"/>
+      <c r="T23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>110</v>
       </c>
       <c r="B24">
         <v>508.7</v>
       </c>
-      <c r="N24">
+      <c r="O24" s="8">
+        <f t="shared" si="0"/>
+        <v>0.15974478289417338</v>
+      </c>
+      <c r="P24">
         <v>508.7</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <v>110</v>
       </c>
-      <c r="Q24" s="3"/>
+      <c r="S24" s="3"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>115</v>
       </c>
       <c r="B25">
         <v>442.6</v>
       </c>
-      <c r="N25">
+      <c r="O25" s="8">
+        <f t="shared" si="0"/>
+        <v>0.13986746595675406</v>
+      </c>
+      <c r="P25">
         <v>442.6</v>
       </c>
-      <c r="O25">
+      <c r="Q25">
         <v>115</v>
       </c>
-      <c r="P25" s="2"/>
-      <c r="Q25" s="3"/>
+      <c r="R25" s="2"/>
+      <c r="S25" s="3"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>120</v>
       </c>
       <c r="B26">
         <v>386.6</v>
       </c>
-      <c r="N26">
+      <c r="O26" s="8">
+        <f t="shared" si="0"/>
+        <v>0.12282941482294495</v>
+      </c>
+      <c r="P26">
         <v>386.6</v>
       </c>
-      <c r="O26">
+      <c r="Q26">
         <v>120</v>
       </c>
-      <c r="P26" s="2"/>
+      <c r="R26" s="2"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>125</v>
       </c>
       <c r="B27">
         <v>338.7</v>
       </c>
-      <c r="N27">
+      <c r="O27" s="8">
+        <f t="shared" si="0"/>
+        <v>0.10810933676380974</v>
+      </c>
+      <c r="P27">
         <v>338.7</v>
       </c>
-      <c r="O27">
+      <c r="Q27">
         <v>125</v>
       </c>
-      <c r="P27" s="2"/>
+      <c r="R27" s="2"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>130</v>
       </c>
       <c r="B28">
         <v>297.7</v>
       </c>
-      <c r="N28">
+      <c r="O28" s="8">
+        <f t="shared" si="0"/>
+        <v>9.5400914767375222E-2</v>
+      </c>
+      <c r="P28">
         <v>297.7</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <v>130</v>
       </c>
-      <c r="P28" s="2"/>
-      <c r="Q28" t="s">
+      <c r="R28" s="2"/>
+      <c r="S28" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>135</v>
       </c>
       <c r="B29">
         <v>262.39999999999998</v>
       </c>
-      <c r="N29">
+      <c r="O29" s="8">
+        <f t="shared" si="0"/>
+        <v>8.4377923292796989E-2</v>
+      </c>
+      <c r="P29">
         <v>262.39999999999998</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <v>135</v>
       </c>
-      <c r="P29" s="2"/>
+      <c r="R29" s="2"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>140</v>
       </c>
       <c r="B30">
         <v>231.9</v>
       </c>
-      <c r="N30">
+      <c r="O30" s="8">
+        <f t="shared" si="0"/>
+        <v>7.4792560521506277E-2</v>
+      </c>
+      <c r="P30">
         <v>231.9</v>
       </c>
-      <c r="O30">
+      <c r="Q30">
         <v>140</v>
       </c>
-      <c r="P30" s="2"/>
+      <c r="R30" s="2"/>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>145</v>
       </c>
       <c r="B31">
         <v>205.5</v>
       </c>
-      <c r="N31">
+      <c r="O31" s="8">
+        <f t="shared" si="0"/>
+        <v>6.6449463524570082E-2</v>
+      </c>
+      <c r="P31">
         <v>205.5</v>
       </c>
-      <c r="O31">
+      <c r="Q31">
         <v>145</v>
       </c>
-      <c r="P31" s="2"/>
+      <c r="R31" s="2"/>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>150</v>
       </c>
       <c r="B32">
         <v>182.6</v>
       </c>
-      <c r="N32">
+      <c r="O32" s="8">
+        <f t="shared" si="0"/>
+        <v>5.9177420305226554E-2</v>
+      </c>
+      <c r="P32">
         <v>182.6</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>150</v>
       </c>
-      <c r="P32" s="2"/>
+      <c r="R32" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>